<commit_message>
Generacion de los recibos y ficheros con excel de la p4 para fecha 1T de 2023
</commit_message>
<xml_diff>
--- a/src/resources/SistemasAgua.xlsx
+++ b/src/resources/SistemasAgua.xlsx
@@ -5,39 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hds_8\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\202898\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA42F524-A6D0-442B-A471-5D24016F1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FF753A-F146-4478-9E33-87A6307BEA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Contribuyente" sheetId="1" r:id="rId1"/>
     <sheet name="Ordenanza" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="509">
   <si>
     <t>Nombre</t>
   </si>
@@ -1452,9 +1441,6 @@
     <t>Pueblo</t>
   </si>
   <si>
-    <t>Prueba</t>
-  </si>
-  <si>
     <t>Hogar</t>
   </si>
   <si>
@@ -1518,36 +1504,24 @@
     <t>SobreQueConcepto</t>
   </si>
   <si>
-    <t>Empresa</t>
-  </si>
-  <si>
     <t>conceptosACobrar</t>
   </si>
   <si>
     <t>1 2 3</t>
   </si>
   <si>
-    <t>1 2</t>
-  </si>
-  <si>
     <t>TipoCalculo</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Importe Desagüe</t>
   </si>
   <si>
     <t>Juan</t>
   </si>
   <si>
-    <t>3 1</t>
-  </si>
-  <si>
     <t>PYME</t>
   </si>
   <si>
@@ -1555,6 +1529,30 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Astorga</t>
+  </si>
+  <si>
+    <t>Cuarto tramo</t>
+  </si>
+  <si>
+    <t>Agua cuarto tramo</t>
+  </si>
+  <si>
+    <t>Gran empresa</t>
+  </si>
+  <si>
+    <t>Precio fijo alcantarillado</t>
+  </si>
+  <si>
+    <t>Importe alcantarillado</t>
+  </si>
+  <si>
+    <t>4 5 10</t>
+  </si>
+  <si>
+    <t>6 8 9</t>
   </si>
 </sst>
 </file>
@@ -1632,9 +1630,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1672,7 +1670,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1778,7 +1776,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1920,7 +1918,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1930,22 +1928,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6ACB8-7F34-425E-9257-91AD8B97F35F}">
   <dimension ref="A1:Q152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" style="7"/>
-    <col min="17" max="17" width="11.44140625" style="1"/>
+    <col min="15" max="15" width="11.42578125" style="7"/>
+    <col min="17" max="17" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1995,12 +1993,12 @@
         <v>266</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B2" t="s">
         <v>95</v>
@@ -2024,7 +2022,7 @@
         <v>267</v>
       </c>
       <c r="K2" t="s">
-        <v>264</v>
+        <v>500</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -2039,10 +2037,10 @@
         <v>45294</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2083,10 +2081,10 @@
         <v>38267</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2127,10 +2125,10 @@
         <v>39682</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2157,7 @@
         <v>264</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M5">
         <v>942</v>
@@ -2171,10 +2169,10 @@
         <v>38765</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2215,10 +2213,10 @@
         <v>38646</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2259,10 +2257,10 @@
         <v>41039</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2291,7 +2289,7 @@
         <v>264</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M8">
         <v>586</v>
@@ -2303,10 +2301,10 @@
         <v>43912</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2347,10 +2345,10 @@
         <v>41745</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2391,10 +2389,10 @@
         <v>44978</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2423,7 +2421,7 @@
         <v>264</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M11">
         <v>645</v>
@@ -2435,10 +2433,10 @@
         <v>39134</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2479,10 +2477,10 @@
         <v>44614</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2523,10 +2521,10 @@
         <v>41490</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2555,7 +2553,7 @@
         <v>264</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M14">
         <v>72</v>
@@ -2567,16 +2565,16 @@
         <v>41228</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2617,10 +2615,10 @@
         <v>40637</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2661,10 +2659,10 @@
         <v>45079</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2705,10 +2703,10 @@
         <v>43017</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2737,7 +2735,7 @@
         <v>264</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M19">
         <v>968</v>
@@ -2749,10 +2747,10 @@
         <v>39371</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2793,10 +2791,10 @@
         <v>39934</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2837,10 +2835,10 @@
         <v>43868</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2866,7 +2864,7 @@
         <v>264</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M22">
         <v>25</v>
@@ -2878,10 +2876,10 @@
         <v>41262</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2919,10 +2917,10 @@
         <v>45279</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2960,10 +2958,10 @@
         <v>39982</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2989,7 +2987,7 @@
         <v>264</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M25">
         <v>799</v>
@@ -3001,16 +2999,16 @@
         <v>41034</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3051,10 +3049,10 @@
         <v>39525</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -3083,7 +3081,7 @@
         <v>264</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M28">
         <v>410</v>
@@ -3095,10 +3093,10 @@
         <v>42667</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -3139,10 +3137,10 @@
         <v>44639</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -3183,10 +3181,10 @@
         <v>37937</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -3227,10 +3225,10 @@
         <v>43242</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3271,28 +3269,28 @@
         <v>39555</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -3321,7 +3319,7 @@
         <v>264</v>
       </c>
       <c r="L36">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M36">
         <v>413</v>
@@ -3333,10 +3331,10 @@
         <v>43230</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -3377,10 +3375,10 @@
         <v>38841</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -3421,10 +3419,10 @@
         <v>44389</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -3465,10 +3463,10 @@
         <v>45242</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -3509,10 +3507,10 @@
         <v>41309</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3553,10 +3551,10 @@
         <v>45142</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -3597,10 +3595,10 @@
         <v>45048</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -3641,10 +3639,10 @@
         <v>44479</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -3685,10 +3683,10 @@
         <v>42624</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -3729,10 +3727,10 @@
         <v>42708</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -3773,10 +3771,10 @@
         <v>44180</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -3817,10 +3815,10 @@
         <v>45047</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -3849,7 +3847,7 @@
         <v>264</v>
       </c>
       <c r="L48">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M48">
         <v>330</v>
@@ -3861,10 +3859,10 @@
         <v>42182</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -3905,10 +3903,10 @@
         <v>43032</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -3949,10 +3947,10 @@
         <v>42490</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -3981,7 +3979,7 @@
         <v>264</v>
       </c>
       <c r="L51">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M51">
         <v>178</v>
@@ -3993,10 +3991,10 @@
         <v>39101</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -4037,10 +4035,10 @@
         <v>44962</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -4081,10 +4079,10 @@
         <v>42148</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -4113,7 +4111,7 @@
         <v>264</v>
       </c>
       <c r="L54">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M54">
         <v>556</v>
@@ -4125,10 +4123,10 @@
         <v>43805</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -4169,34 +4167,34 @@
         <v>40575</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="4"/>
       <c r="F56" s="6"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="E57" s="4"/>
       <c r="F57" s="6"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="E58" s="4"/>
       <c r="F58" s="6"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="E59" s="4"/>
       <c r="F59" s="6"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -4237,10 +4235,10 @@
         <v>38607</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>54</v>
       </c>
@@ -4281,10 +4279,10 @@
         <v>42083</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>21</v>
       </c>
@@ -4313,7 +4311,7 @@
         <v>264</v>
       </c>
       <c r="L62">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M62">
         <v>446</v>
@@ -4325,10 +4323,10 @@
         <v>39105</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -4369,10 +4367,10 @@
         <v>41938</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -4410,10 +4408,10 @@
         <v>43691</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -4451,10 +4449,10 @@
         <v>42810</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -4492,10 +4490,10 @@
         <v>45570</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>25</v>
       </c>
@@ -4536,10 +4534,10 @@
         <v>40799</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -4580,10 +4578,10 @@
         <v>42926</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>27</v>
       </c>
@@ -4612,7 +4610,7 @@
         <v>264</v>
       </c>
       <c r="L69">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M69">
         <v>983</v>
@@ -4624,10 +4622,10 @@
         <v>43569</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -4668,10 +4666,10 @@
         <v>42657</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -4712,10 +4710,10 @@
         <v>38841</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -4756,10 +4754,10 @@
         <v>42522</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -4800,10 +4798,10 @@
         <v>39748</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>56</v>
       </c>
@@ -4832,7 +4830,7 @@
         <v>264</v>
       </c>
       <c r="L74">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M74">
         <v>545</v>
@@ -4844,10 +4842,10 @@
         <v>40427</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>57</v>
       </c>
@@ -4888,10 +4886,10 @@
         <v>42543</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>58</v>
       </c>
@@ -4932,10 +4930,10 @@
         <v>45341</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>59</v>
       </c>
@@ -4976,16 +4974,16 @@
         <v>39295</v>
       </c>
       <c r="Q77" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D78" s="1"/>
       <c r="E78" s="4"/>
       <c r="F78" s="6"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>60</v>
       </c>
@@ -5026,10 +5024,10 @@
         <v>38315</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>61</v>
       </c>
@@ -5058,7 +5056,7 @@
         <v>264</v>
       </c>
       <c r="L80">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M80">
         <v>692</v>
@@ -5070,10 +5068,10 @@
         <v>43991</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>62</v>
       </c>
@@ -5114,10 +5112,10 @@
         <v>45030</v>
       </c>
       <c r="Q81" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>63</v>
       </c>
@@ -5158,10 +5156,10 @@
         <v>40558</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>64</v>
       </c>
@@ -5202,10 +5200,10 @@
         <v>42650</v>
       </c>
       <c r="Q83" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>65</v>
       </c>
@@ -5243,16 +5241,16 @@
         <v>41024</v>
       </c>
       <c r="Q84" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D85" s="1"/>
       <c r="E85" s="4"/>
       <c r="F85" s="6"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>66</v>
       </c>
@@ -5281,7 +5279,7 @@
         <v>264</v>
       </c>
       <c r="L86">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M86">
         <v>597</v>
@@ -5293,10 +5291,10 @@
         <v>45627</v>
       </c>
       <c r="Q86" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>67</v>
       </c>
@@ -5337,10 +5335,10 @@
         <v>39308</v>
       </c>
       <c r="Q87" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>68</v>
       </c>
@@ -5381,10 +5379,10 @@
         <v>40028</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>69</v>
       </c>
@@ -5425,10 +5423,10 @@
         <v>39734</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>52</v>
       </c>
@@ -5466,10 +5464,10 @@
         <v>40418</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -5510,10 +5508,10 @@
         <v>39480</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>71</v>
       </c>
@@ -5554,10 +5552,10 @@
         <v>39939</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -5586,7 +5584,7 @@
         <v>264</v>
       </c>
       <c r="L93">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M93">
         <v>76</v>
@@ -5598,10 +5596,10 @@
         <v>41007</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>73</v>
       </c>
@@ -5640,10 +5638,10 @@
         <v>41247</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>74</v>
       </c>
@@ -5684,46 +5682,46 @@
         <v>45099</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
       <c r="F96" s="6"/>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D97" s="1"/>
       <c r="E97" s="4"/>
       <c r="F97" s="6"/>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
       <c r="E98" s="4"/>
       <c r="F98" s="6"/>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>
       <c r="E99" s="4"/>
       <c r="F99" s="6"/>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
       <c r="E100" s="4"/>
       <c r="F100" s="6"/>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D101" s="1"/>
       <c r="E101" s="4"/>
       <c r="F101" s="6"/>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>56</v>
       </c>
@@ -5764,10 +5762,10 @@
         <v>40726</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>57</v>
       </c>
@@ -5796,7 +5794,7 @@
         <v>264</v>
       </c>
       <c r="L103">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M103">
         <v>964</v>
@@ -5808,10 +5806,10 @@
         <v>44937</v>
       </c>
       <c r="Q103" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>58</v>
       </c>
@@ -5852,10 +5850,10 @@
         <v>40195</v>
       </c>
       <c r="Q104" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>59</v>
       </c>
@@ -5896,10 +5894,10 @@
         <v>40974</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -5928,7 +5926,7 @@
         <v>264</v>
       </c>
       <c r="L106">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M106">
         <v>188</v>
@@ -5940,130 +5938,130 @@
         <v>44615</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D107" s="1"/>
       <c r="E107" s="4"/>
       <c r="F107" s="6"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D108" s="1"/>
       <c r="E108" s="4"/>
       <c r="F108" s="6"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D109" s="1"/>
       <c r="E109" s="4"/>
       <c r="F109" s="6"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
       <c r="F110" s="6"/>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
       <c r="E111" s="4"/>
       <c r="F111" s="6"/>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
       <c r="F112" s="6"/>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D113" s="1"/>
       <c r="E113" s="4"/>
       <c r="F113" s="6"/>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D114" s="1"/>
       <c r="E114" s="4"/>
       <c r="F114" s="6"/>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D115" s="1"/>
       <c r="E115" s="4"/>
       <c r="F115" s="6"/>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D116" s="1"/>
       <c r="E116" s="4"/>
       <c r="F116" s="6"/>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D117" s="1"/>
       <c r="E117" s="4"/>
       <c r="F117" s="6"/>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D118" s="1"/>
       <c r="E118" s="4"/>
       <c r="F118" s="6"/>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D119" s="1"/>
       <c r="E119" s="4"/>
       <c r="F119" s="6"/>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D120" s="1"/>
       <c r="E120" s="4"/>
       <c r="F120" s="6"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
       <c r="E121" s="4"/>
       <c r="F121" s="6"/>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D122" s="1"/>
       <c r="E122" s="4"/>
       <c r="F122" s="6"/>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D123" s="1"/>
       <c r="E123" s="4"/>
       <c r="F123" s="6"/>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
       <c r="E124" s="4"/>
       <c r="F124" s="6"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D125" s="1"/>
       <c r="E125" s="4"/>
       <c r="F125" s="6"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D126" s="1"/>
       <c r="E126" s="4"/>
       <c r="F126" s="6"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>75</v>
       </c>
@@ -6104,10 +6102,10 @@
         <v>39738</v>
       </c>
       <c r="Q127" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>76</v>
       </c>
@@ -6148,10 +6146,10 @@
         <v>40453</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>77</v>
       </c>
@@ -6192,10 +6190,10 @@
         <v>43473</v>
       </c>
       <c r="Q129" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>68</v>
       </c>
@@ -6224,7 +6222,7 @@
         <v>264</v>
       </c>
       <c r="L130">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M130">
         <v>1</v>
@@ -6236,10 +6234,10 @@
         <v>40935</v>
       </c>
       <c r="Q130" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>69</v>
       </c>
@@ -6280,10 +6278,10 @@
         <v>44175</v>
       </c>
       <c r="Q131" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>52</v>
       </c>
@@ -6309,7 +6307,7 @@
         <v>357</v>
       </c>
       <c r="K132" t="s">
-        <v>264</v>
+        <v>500</v>
       </c>
       <c r="L132">
         <v>0</v>
@@ -6324,10 +6322,10 @@
         <v>40887</v>
       </c>
       <c r="Q132" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>70</v>
       </c>
@@ -6368,10 +6366,10 @@
         <v>43334</v>
       </c>
       <c r="Q133" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>71</v>
       </c>
@@ -6400,7 +6398,7 @@
         <v>264</v>
       </c>
       <c r="L134">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M134">
         <v>728</v>
@@ -6412,10 +6410,10 @@
         <v>42557</v>
       </c>
       <c r="Q134" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>72</v>
       </c>
@@ -6454,10 +6452,10 @@
         <v>43929</v>
       </c>
       <c r="Q135" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>73</v>
       </c>
@@ -6498,69 +6496,69 @@
         <v>40457</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E137" s="4"/>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E138" s="4"/>
       <c r="F138" s="6"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E139" s="4"/>
       <c r="F139" s="6"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E140" s="4"/>
       <c r="F140" s="6"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E141" s="4"/>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E142" s="4"/>
       <c r="F142" s="6"/>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E143" s="4"/>
       <c r="F143" s="6"/>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E144" s="4"/>
       <c r="F144" s="6"/>
     </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E145" s="4"/>
       <c r="F145" s="6"/>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E146" s="4"/>
       <c r="F146" s="6"/>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E147" s="4"/>
       <c r="F147" s="6"/>
     </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E148" s="4"/>
       <c r="F148" s="6"/>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E149" s="4"/>
       <c r="F149" s="6"/>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E150" s="4"/>
       <c r="F150" s="6"/>
     </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F151" s="6"/>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F152" s="6"/>
     </row>
   </sheetData>
@@ -6571,80 +6569,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="46" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="11" max="12" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>470</v>
       </c>
       <c r="B1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C1" t="s">
         <v>469</v>
       </c>
       <c r="D1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>474</v>
-      </c>
-      <c r="F1" t="s">
-        <v>475</v>
       </c>
       <c r="G1" t="s">
         <v>467</v>
       </c>
       <c r="H1" t="s">
+        <v>475</v>
+      </c>
+      <c r="I1" t="s">
         <v>476</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>477</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>478</v>
       </c>
-      <c r="K1" t="s">
-        <v>479</v>
-      </c>
       <c r="L1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B2" t="s">
         <v>471</v>
-      </c>
-      <c r="B2" t="s">
-        <v>472</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E2" t="s">
         <v>480</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>481</v>
-      </c>
-      <c r="F2" t="s">
-        <v>482</v>
       </c>
       <c r="G2" t="s">
         <v>264</v>
@@ -6659,24 +6657,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B3" t="s">
         <v>471</v>
-      </c>
-      <c r="B3" t="s">
-        <v>472</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E3" t="s">
+        <v>482</v>
+      </c>
+      <c r="F3" t="s">
         <v>483</v>
-      </c>
-      <c r="F3" t="s">
-        <v>484</v>
       </c>
       <c r="G3" t="s">
         <v>264</v>
@@ -6691,24 +6689,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>501</v>
+      </c>
+      <c r="B4" t="s">
         <v>471</v>
-      </c>
-      <c r="B4" t="s">
-        <v>472</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E4" t="s">
+        <v>484</v>
+      </c>
+      <c r="F4" t="s">
         <v>485</v>
-      </c>
-      <c r="F4" t="s">
-        <v>486</v>
       </c>
       <c r="G4" t="s">
         <v>264</v>
@@ -6723,219 +6721,460 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B5" t="s">
         <v>471</v>
-      </c>
-      <c r="B5" t="s">
-        <v>472</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E5" t="s">
+        <v>486</v>
+      </c>
+      <c r="F5" t="s">
         <v>487</v>
       </c>
-      <c r="F5" t="s">
-        <v>488</v>
-      </c>
       <c r="G5" t="s">
         <v>264</v>
       </c>
       <c r="I5">
-        <v>9999</v>
+        <v>100</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>501</v>
+      </c>
+      <c r="B6" t="s">
         <v>471</v>
       </c>
-      <c r="B6" t="s">
-        <v>472</v>
-      </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>479</v>
+      </c>
+      <c r="E6" t="s">
+        <v>502</v>
+      </c>
+      <c r="F6" t="s">
+        <v>503</v>
+      </c>
+      <c r="G6" t="s">
+        <v>264</v>
+      </c>
+      <c r="I6">
+        <v>9999</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>501</v>
+      </c>
+      <c r="B7" t="s">
+        <v>471</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
+        <v>488</v>
+      </c>
+      <c r="E7" t="s">
+        <v>480</v>
+      </c>
+      <c r="F7" t="s">
         <v>489</v>
-      </c>
-      <c r="E6" t="s">
-        <v>481</v>
-      </c>
-      <c r="F6" t="s">
-        <v>490</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>471</v>
-      </c>
-      <c r="B7" t="s">
-        <v>472</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>491</v>
-      </c>
-      <c r="E7" t="s">
-        <v>491</v>
-      </c>
-      <c r="F7" t="s">
-        <v>500</v>
       </c>
       <c r="K7">
         <v>10</v>
       </c>
       <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>501</v>
+      </c>
+      <c r="B8" t="s">
+        <v>471</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>490</v>
+      </c>
+      <c r="E8" t="s">
+        <v>490</v>
+      </c>
+      <c r="F8" t="s">
+        <v>496</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>471</v>
-      </c>
-      <c r="B8" t="s">
-        <v>493</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>480</v>
-      </c>
-      <c r="E8" t="s">
-        <v>481</v>
-      </c>
-      <c r="F8" t="s">
-        <v>482</v>
-      </c>
-      <c r="G8" t="s">
-        <v>264</v>
-      </c>
-      <c r="H8">
-        <v>50</v>
-      </c>
-      <c r="I8">
-        <v>20</v>
-      </c>
       <c r="M8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B9" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9" t="s">
+        <v>479</v>
+      </c>
+      <c r="E9" t="s">
         <v>480</v>
       </c>
-      <c r="E9" t="s">
-        <v>483</v>
-      </c>
       <c r="F9" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G9" t="s">
-        <v>264</v>
+        <v>500</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
       </c>
       <c r="I9">
-        <v>9999</v>
-      </c>
-      <c r="J9">
-        <v>0.75</v>
+        <v>20</v>
       </c>
       <c r="M9">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B10" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="E10" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F10" t="s">
-        <v>490</v>
-      </c>
-      <c r="H10">
-        <v>25</v>
+        <v>483</v>
+      </c>
+      <c r="G10" t="s">
+        <v>500</v>
+      </c>
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B11" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E11" t="s">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="F11" t="s">
-        <v>504</v>
+        <v>485</v>
       </c>
       <c r="G11" t="s">
-        <v>505</v>
-      </c>
-      <c r="H11">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="I11">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J11">
         <v>2</v>
       </c>
       <c r="M11">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>501</v>
+      </c>
+      <c r="B12" t="s">
+        <v>504</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>479</v>
+      </c>
+      <c r="E12" t="s">
+        <v>486</v>
+      </c>
+      <c r="F12" t="s">
+        <v>487</v>
+      </c>
+      <c r="G12" t="s">
+        <v>500</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>501</v>
+      </c>
+      <c r="B13" t="s">
+        <v>504</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>479</v>
+      </c>
+      <c r="E13" t="s">
+        <v>502</v>
+      </c>
+      <c r="F13" t="s">
+        <v>503</v>
+      </c>
+      <c r="G13" t="s">
+        <v>500</v>
+      </c>
+      <c r="I13">
+        <v>9999</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>501</v>
+      </c>
+      <c r="B14" t="s">
+        <v>504</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>490</v>
+      </c>
+      <c r="E14" t="s">
+        <v>480</v>
+      </c>
+      <c r="F14" t="s">
+        <v>489</v>
+      </c>
+      <c r="H14">
+        <v>25</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>501</v>
+      </c>
+      <c r="B15" t="s">
+        <v>498</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>479</v>
+      </c>
+      <c r="E15" t="s">
+        <v>472</v>
+      </c>
+      <c r="F15" t="s">
+        <v>499</v>
+      </c>
+      <c r="G15" t="s">
+        <v>500</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>501</v>
+      </c>
+      <c r="B16" t="s">
+        <v>471</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>490</v>
+      </c>
+      <c r="E16" t="s">
+        <v>490</v>
+      </c>
+      <c r="F16" t="s">
+        <v>496</v>
+      </c>
+      <c r="K16">
+        <v>10</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>501</v>
+      </c>
+      <c r="B17" t="s">
+        <v>498</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>488</v>
+      </c>
+      <c r="E17" t="s">
+        <v>480</v>
+      </c>
+      <c r="F17" t="s">
+        <v>505</v>
+      </c>
+      <c r="H17">
+        <v>30</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>501</v>
+      </c>
+      <c r="B18" t="s">
+        <v>498</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>490</v>
+      </c>
+      <c r="E18" t="s">
+        <v>490</v>
+      </c>
+      <c r="F18" t="s">
+        <v>496</v>
+      </c>
+      <c r="K18">
+        <v>20</v>
+      </c>
+      <c r="L18">
+        <v>9</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>501</v>
+      </c>
+      <c r="B19" t="s">
+        <v>504</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>488</v>
+      </c>
+      <c r="E19" t="s">
+        <v>480</v>
+      </c>
+      <c r="F19" t="s">
+        <v>506</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>